<commit_message>
Write up for Churn Project - In Progress
</commit_message>
<xml_diff>
--- a/Code/Telecom_Customer_Churn_Prediction/results_final.xlsx
+++ b/Code/Telecom_Customer_Churn_Prediction/results_final.xlsx
@@ -52,16 +52,16 @@
     <t>StackingCV</t>
   </si>
   <si>
+    <t>Random Forest</t>
+  </si>
+  <si>
+    <t>XGB</t>
+  </si>
+  <si>
+    <t>Voting</t>
+  </si>
+  <si>
     <t>Stacking (SGD)</t>
-  </si>
-  <si>
-    <t>Random Forest</t>
-  </si>
-  <si>
-    <t>Voting</t>
-  </si>
-  <si>
-    <t>XGB</t>
   </si>
   <si>
     <t>Stacking (SVC)</t>
@@ -510,33 +510,33 @@
         <v>26</v>
       </c>
       <c r="E2">
-        <v>0.9732458354366481</v>
+        <v>0.9742554265522464</v>
       </c>
       <c r="F2">
-        <v>0.9675126903553299</v>
+        <v>0.9634517766497462</v>
       </c>
       <c r="G2">
-        <v>0.9784394250513347</v>
+        <v>0.9844398340248963</v>
       </c>
       <c r="H2">
-        <v>0.9960960593643611</v>
+        <v>0.9937435019264876</v>
       </c>
       <c r="I2">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="J2">
-        <v>975</v>
+        <v>981</v>
       </c>
       <c r="K2">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L2">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -548,33 +548,33 @@
         <v>26</v>
       </c>
       <c r="E3">
-        <v>0.9727410398788491</v>
+        <v>0.9581019687026754</v>
       </c>
       <c r="F3">
-        <v>0.965482233502538</v>
+        <v>0.9461928934010152</v>
       </c>
       <c r="G3">
-        <v>0.9794026776519053</v>
+        <v>0.9688149688149689</v>
       </c>
       <c r="H3">
-        <v>0.9956964915499561</v>
+        <v>0.9925932155016003</v>
       </c>
       <c r="I3">
-        <v>951</v>
+        <v>932</v>
       </c>
       <c r="J3">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="K3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L3">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -586,28 +586,28 @@
         <v>26</v>
       </c>
       <c r="E4">
-        <v>0.956082786471479</v>
+        <v>0.9727410398788491</v>
       </c>
       <c r="F4">
-        <v>0.9512690355329949</v>
+        <v>0.9614213197969543</v>
       </c>
       <c r="G4">
-        <v>0.9600409836065574</v>
+        <v>0.9833852544132918</v>
       </c>
       <c r="H4">
-        <v>0.9941904674535706</v>
+        <v>0.9923888447189774</v>
       </c>
       <c r="I4">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="J4">
-        <v>957</v>
+        <v>980</v>
       </c>
       <c r="K4">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="L4">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -624,33 +624,33 @@
         <v>26</v>
       </c>
       <c r="E5">
-        <v>0.9565875820292782</v>
+        <v>0.9540636042402827</v>
       </c>
       <c r="F5">
-        <v>0.9512690355329949</v>
+        <v>0.9451776649746193</v>
       </c>
       <c r="G5">
-        <v>0.961025641025641</v>
+        <v>0.9617768595041323</v>
       </c>
       <c r="H5">
-        <v>0.9937129227570179</v>
+        <v>0.9912370293356166</v>
       </c>
       <c r="I5">
-        <v>937</v>
+        <v>931</v>
       </c>
       <c r="J5">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="K5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L5">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -662,28 +662,28 @@
         <v>26</v>
       </c>
       <c r="E6">
-        <v>0.9722362443210499</v>
+        <v>0.9742554265522464</v>
       </c>
       <c r="F6">
-        <v>0.9634517766497462</v>
+        <v>0.9644670050761421</v>
       </c>
       <c r="G6">
-        <v>0.9803719008264463</v>
+        <v>0.9834368530020704</v>
       </c>
       <c r="H6">
-        <v>0.9934642121786639</v>
+        <v>0.9879997145944183</v>
       </c>
       <c r="I6">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="J6">
-        <v>977</v>
+        <v>980</v>
       </c>
       <c r="K6">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L6">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -700,28 +700,28 @@
         <v>26</v>
       </c>
       <c r="E7">
-        <v>0.9702170620898536</v>
+        <v>0.9727410398788491</v>
       </c>
       <c r="F7">
-        <v>0.9593908629441624</v>
+        <v>0.9604060913705583</v>
       </c>
       <c r="G7">
-        <v>0.9802904564315352</v>
+        <v>0.9843912591050988</v>
       </c>
       <c r="H7">
-        <v>0.9775314455792714</v>
+        <v>0.9760279697470082</v>
       </c>
       <c r="I7">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="J7">
-        <v>977</v>
+        <v>981</v>
       </c>
       <c r="K7">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L7">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -738,28 +738,28 @@
         <v>26</v>
       </c>
       <c r="E8">
-        <v>0.9515396264512872</v>
+        <v>0.9570923775870772</v>
       </c>
       <c r="F8">
-        <v>0.9573604060913705</v>
+        <v>0.950253807106599</v>
       </c>
       <c r="G8">
-        <v>0.9458375125376128</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="H8">
-        <v>0.9515717693107455</v>
+        <v>0.9570546143966729</v>
       </c>
       <c r="I8">
-        <v>943</v>
+        <v>936</v>
       </c>
       <c r="J8">
-        <v>942</v>
+        <v>960</v>
       </c>
       <c r="K8">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="L8">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -776,28 +776,28 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <v>0.8571428571428571</v>
+        <v>0.8642099949520444</v>
       </c>
       <c r="F9">
-        <v>0.8791878172588833</v>
+        <v>0.8812182741116751</v>
       </c>
       <c r="G9">
-        <v>0.8407766990291262</v>
+        <v>0.8509803921568627</v>
       </c>
       <c r="H9">
-        <v>0.9136270972213729</v>
+        <v>0.9167273153527817</v>
       </c>
       <c r="I9">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="J9">
-        <v>832</v>
+        <v>844</v>
       </c>
       <c r="K9">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="L9">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -814,28 +814,28 @@
         <v>27</v>
       </c>
       <c r="E10">
-        <v>0.9126703685007572</v>
+        <v>0.9121655729429581</v>
       </c>
       <c r="F10">
-        <v>0.9238578680203046</v>
+        <v>0.9218274111675127</v>
       </c>
       <c r="G10">
-        <v>0.9027777777777778</v>
+        <v>0.9034825870646767</v>
       </c>
       <c r="H10">
-        <v>0.9127321468615579</v>
+        <v>0.9122189264672904</v>
       </c>
       <c r="I10">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="J10">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="K10">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L10">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -852,28 +852,28 @@
         <v>26</v>
       </c>
       <c r="E11">
-        <v>0.8970217062089854</v>
+        <v>0.9040888440181727</v>
       </c>
       <c r="F11">
-        <v>0.8964467005076142</v>
+        <v>0.9045685279187817</v>
       </c>
       <c r="G11">
-        <v>0.8964467005076142</v>
+        <v>0.9027355623100304</v>
       </c>
       <c r="H11">
-        <v>0.8970185309766987</v>
+        <v>0.9043870915132611</v>
       </c>
       <c r="I11">
-        <v>883</v>
+        <v>891</v>
       </c>
       <c r="J11">
-        <v>894</v>
+        <v>900</v>
       </c>
       <c r="K11">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="L11">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -890,28 +890,28 @@
         <v>27</v>
       </c>
       <c r="E12">
-        <v>0.8086824835941444</v>
+        <v>0.8182735991923271</v>
       </c>
       <c r="F12">
-        <v>0.7553299492385787</v>
+        <v>0.7756345177664975</v>
       </c>
       <c r="G12">
-        <v>0.8435374149659864</v>
+        <v>0.8460686600221484</v>
       </c>
       <c r="H12">
-        <v>0.8476199213096041</v>
+        <v>0.8563553707214646</v>
       </c>
       <c r="I12">
-        <v>744</v>
+        <v>764</v>
       </c>
       <c r="J12">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="K12">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L12">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -928,28 +928,28 @@
         <v>27</v>
       </c>
       <c r="E13">
-        <v>0.790005047955578</v>
+        <v>0.7895002523977789</v>
       </c>
       <c r="F13">
-        <v>0.8</v>
+        <v>0.8040609137055837</v>
       </c>
       <c r="G13">
-        <v>0.7825223435948362</v>
+        <v>0.7795275590551181</v>
       </c>
       <c r="H13">
-        <v>0.8375002548264122</v>
+        <v>0.8407406274845576</v>
       </c>
       <c r="I13">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="J13">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="K13">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="L13">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -966,19 +966,19 @@
         <v>27</v>
       </c>
       <c r="E14">
-        <v>0.6335184250378597</v>
+        <v>0.6456335184250379</v>
       </c>
       <c r="F14">
-        <v>0.8426395939086294</v>
+        <v>0.867005076142132</v>
       </c>
       <c r="G14">
-        <v>0.5924339757316203</v>
+        <v>0.5992982456140351</v>
       </c>
       <c r="H14">
-        <v>0.6954457423603042</v>
+        <v>0.7009061627219538</v>
       </c>
       <c r="I14">
-        <v>830</v>
+        <v>854</v>
       </c>
       <c r="J14">
         <v>425</v>
@@ -987,7 +987,7 @@
         <v>571</v>
       </c>
       <c r="L14">
-        <v>155</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>